<commit_message>
Updated results using celtra server
</commit_message>
<xml_diff>
--- a/results/comparison.xlsx
+++ b/results/comparison.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24700" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27100" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>Method/example</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Partial Avg</t>
+  </si>
+  <si>
+    <t>Max score</t>
+  </si>
+  <si>
+    <t>11 (same as 5, but 30000 length)</t>
   </si>
 </sst>
 </file>
@@ -116,8 +122,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -132,15 +160,37 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -470,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -556,9 +606,15 @@
       <c r="J4">
         <v>568</v>
       </c>
+      <c r="K4">
+        <v>297</v>
+      </c>
+      <c r="L4">
+        <v>388</v>
+      </c>
       <c r="M4" s="2">
         <f>AVERAGE(H4:L4)</f>
-        <v>642</v>
+        <v>522.20000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -593,9 +649,15 @@
       <c r="J5">
         <v>555</v>
       </c>
+      <c r="K5">
+        <v>402</v>
+      </c>
+      <c r="L5">
+        <v>401</v>
+      </c>
       <c r="M5" s="2">
         <f t="shared" ref="M5:M13" si="1">AVERAGE(H5:L5)</f>
-        <v>651.66666666666663</v>
+        <v>551.6</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -630,9 +692,15 @@
       <c r="J6">
         <v>542</v>
       </c>
+      <c r="K6">
+        <v>409</v>
+      </c>
+      <c r="L6">
+        <v>397</v>
+      </c>
       <c r="M6" s="2">
         <f t="shared" si="1"/>
-        <v>646</v>
+        <v>548.79999999999995</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -667,9 +735,15 @@
       <c r="J7">
         <v>455</v>
       </c>
+      <c r="K7">
+        <v>382</v>
+      </c>
+      <c r="L7">
+        <v>391</v>
+      </c>
       <c r="M7" s="2">
         <f t="shared" si="1"/>
-        <v>607.66666666666663</v>
+        <v>519.20000000000005</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -704,9 +778,15 @@
       <c r="J8">
         <v>446</v>
       </c>
+      <c r="K8">
+        <v>403</v>
+      </c>
+      <c r="L8">
+        <v>390</v>
+      </c>
       <c r="M8" s="2">
         <f t="shared" si="1"/>
-        <v>599.33333333333337</v>
+        <v>518.20000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -741,9 +821,15 @@
       <c r="J9">
         <v>430</v>
       </c>
+      <c r="K9">
+        <v>322</v>
+      </c>
+      <c r="L9">
+        <v>409</v>
+      </c>
       <c r="M9" s="2">
         <f t="shared" si="1"/>
-        <v>582.66666666666663</v>
+        <v>495.8</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -778,9 +864,15 @@
       <c r="J10">
         <v>483</v>
       </c>
+      <c r="K10">
+        <v>402</v>
+      </c>
+      <c r="L10">
+        <v>411</v>
+      </c>
       <c r="M10" s="2">
         <f t="shared" si="1"/>
-        <v>589.66666666666663</v>
+        <v>516.4</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -815,9 +907,15 @@
       <c r="J11">
         <v>573</v>
       </c>
+      <c r="K11">
+        <v>386</v>
+      </c>
+      <c r="L11">
+        <v>417</v>
+      </c>
       <c r="M11" s="2">
         <f t="shared" si="1"/>
-        <v>660.66666666666663</v>
+        <v>557</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -852,9 +950,15 @@
       <c r="J12">
         <v>562</v>
       </c>
+      <c r="K12">
+        <v>399</v>
+      </c>
+      <c r="L12">
+        <v>435</v>
+      </c>
       <c r="M12" s="2">
         <f t="shared" si="1"/>
-        <v>659.66666666666663</v>
+        <v>562.6</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -889,9 +993,935 @@
       <c r="J13">
         <v>533</v>
       </c>
+      <c r="K13">
+        <v>391</v>
+      </c>
+      <c r="L13">
+        <v>421</v>
+      </c>
       <c r="M13" s="2">
         <f t="shared" si="1"/>
-        <v>629.66666666666663</v>
+        <v>540.20000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="H20">
+        <v>6</v>
+      </c>
+      <c r="I20">
+        <v>7</v>
+      </c>
+      <c r="J20">
+        <v>8</v>
+      </c>
+      <c r="K20">
+        <v>9</v>
+      </c>
+      <c r="L20">
+        <v>10</v>
+      </c>
+      <c r="N20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>280.95</v>
+      </c>
+      <c r="C21">
+        <v>242</v>
+      </c>
+      <c r="D21">
+        <v>164</v>
+      </c>
+      <c r="E21">
+        <v>211</v>
+      </c>
+      <c r="F21">
+        <v>104</v>
+      </c>
+      <c r="H21">
+        <v>555</v>
+      </c>
+      <c r="I21">
+        <v>432</v>
+      </c>
+      <c r="J21">
+        <v>568</v>
+      </c>
+      <c r="K21">
+        <v>297</v>
+      </c>
+      <c r="L21">
+        <v>388</v>
+      </c>
+      <c r="M21" s="2">
+        <f>SUM(B21:L21)</f>
+        <v>3241.95</v>
+      </c>
+      <c r="N21">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>286.7</v>
+      </c>
+      <c r="C22">
+        <v>265</v>
+      </c>
+      <c r="D22">
+        <v>174</v>
+      </c>
+      <c r="E22">
+        <v>208</v>
+      </c>
+      <c r="F22">
+        <v>102</v>
+      </c>
+      <c r="H22">
+        <v>548</v>
+      </c>
+      <c r="I22">
+        <v>483</v>
+      </c>
+      <c r="J22">
+        <v>555</v>
+      </c>
+      <c r="K22">
+        <v>402</v>
+      </c>
+      <c r="L22">
+        <v>401</v>
+      </c>
+      <c r="M22" s="2">
+        <f t="shared" ref="M22:M32" si="2">SUM(B22:L22)</f>
+        <v>3424.7</v>
+      </c>
+      <c r="N22">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>288.05</v>
+      </c>
+      <c r="C23">
+        <v>257</v>
+      </c>
+      <c r="D23">
+        <v>177</v>
+      </c>
+      <c r="E23">
+        <v>213</v>
+      </c>
+      <c r="F23">
+        <v>102</v>
+      </c>
+      <c r="H23">
+        <v>561</v>
+      </c>
+      <c r="I23">
+        <v>475</v>
+      </c>
+      <c r="J23">
+        <v>542</v>
+      </c>
+      <c r="K23">
+        <v>409</v>
+      </c>
+      <c r="L23">
+        <v>397</v>
+      </c>
+      <c r="M23" s="2">
+        <f t="shared" si="2"/>
+        <v>3421.05</v>
+      </c>
+      <c r="N23">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>286.64999999999998</v>
+      </c>
+      <c r="C24">
+        <v>262</v>
+      </c>
+      <c r="D24">
+        <v>174</v>
+      </c>
+      <c r="E24">
+        <v>213</v>
+      </c>
+      <c r="F24">
+        <v>105</v>
+      </c>
+      <c r="H24">
+        <v>548</v>
+      </c>
+      <c r="I24">
+        <v>459</v>
+      </c>
+      <c r="J24">
+        <v>455</v>
+      </c>
+      <c r="K24">
+        <v>382</v>
+      </c>
+      <c r="L24">
+        <v>391</v>
+      </c>
+      <c r="M24" s="2">
+        <f t="shared" si="2"/>
+        <v>3275.65</v>
+      </c>
+      <c r="N24">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>287.85000000000002</v>
+      </c>
+      <c r="C25">
+        <v>257</v>
+      </c>
+      <c r="D25">
+        <v>175</v>
+      </c>
+      <c r="E25">
+        <v>212</v>
+      </c>
+      <c r="F25">
+        <v>105</v>
+      </c>
+      <c r="H25">
+        <v>546</v>
+      </c>
+      <c r="I25">
+        <v>450</v>
+      </c>
+      <c r="J25">
+        <v>446</v>
+      </c>
+      <c r="K25">
+        <v>403</v>
+      </c>
+      <c r="L25">
+        <v>390</v>
+      </c>
+      <c r="M25" s="2">
+        <f t="shared" si="2"/>
+        <v>3271.85</v>
+      </c>
+      <c r="N25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>286.7</v>
+      </c>
+      <c r="C26">
+        <v>258</v>
+      </c>
+      <c r="D26">
+        <v>169</v>
+      </c>
+      <c r="E26">
+        <v>210</v>
+      </c>
+      <c r="F26">
+        <v>106</v>
+      </c>
+      <c r="H26">
+        <v>537</v>
+      </c>
+      <c r="I26">
+        <v>435</v>
+      </c>
+      <c r="J26">
+        <v>430</v>
+      </c>
+      <c r="K26">
+        <v>322</v>
+      </c>
+      <c r="L26">
+        <v>409</v>
+      </c>
+      <c r="M26" s="2">
+        <f t="shared" si="2"/>
+        <v>3162.7</v>
+      </c>
+      <c r="N26">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27">
+        <v>290.7</v>
+      </c>
+      <c r="C27">
+        <v>289</v>
+      </c>
+      <c r="D27">
+        <v>181</v>
+      </c>
+      <c r="E27">
+        <v>220</v>
+      </c>
+      <c r="F27">
+        <v>104</v>
+      </c>
+      <c r="H27">
+        <v>518</v>
+      </c>
+      <c r="I27">
+        <v>427</v>
+      </c>
+      <c r="J27">
+        <v>483</v>
+      </c>
+      <c r="K27">
+        <v>402</v>
+      </c>
+      <c r="L27">
+        <v>411</v>
+      </c>
+      <c r="M27" s="2">
+        <f t="shared" si="2"/>
+        <v>3325.7</v>
+      </c>
+      <c r="N27">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <v>283.35000000000002</v>
+      </c>
+      <c r="C28">
+        <v>263</v>
+      </c>
+      <c r="D28">
+        <v>169</v>
+      </c>
+      <c r="E28">
+        <v>212</v>
+      </c>
+      <c r="F28">
+        <v>105</v>
+      </c>
+      <c r="H28">
+        <v>567</v>
+      </c>
+      <c r="I28">
+        <v>470</v>
+      </c>
+      <c r="J28">
+        <v>573</v>
+      </c>
+      <c r="K28">
+        <v>386</v>
+      </c>
+      <c r="L28">
+        <v>417</v>
+      </c>
+      <c r="M28" s="2">
+        <f t="shared" si="2"/>
+        <v>3445.35</v>
+      </c>
+      <c r="N28">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <v>287.8</v>
+      </c>
+      <c r="C29">
+        <v>274</v>
+      </c>
+      <c r="D29">
+        <v>171</v>
+      </c>
+      <c r="E29">
+        <v>210</v>
+      </c>
+      <c r="F29">
+        <v>99</v>
+      </c>
+      <c r="H29">
+        <v>572</v>
+      </c>
+      <c r="I29">
+        <v>470</v>
+      </c>
+      <c r="J29">
+        <v>562</v>
+      </c>
+      <c r="K29">
+        <v>399</v>
+      </c>
+      <c r="L29">
+        <v>435</v>
+      </c>
+      <c r="M29" s="2">
+        <f t="shared" si="2"/>
+        <v>3479.8</v>
+      </c>
+      <c r="N29">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30">
+        <v>286.85000000000002</v>
+      </c>
+      <c r="C30">
+        <v>279</v>
+      </c>
+      <c r="D30">
+        <v>176</v>
+      </c>
+      <c r="E30">
+        <v>210</v>
+      </c>
+      <c r="F30">
+        <v>104</v>
+      </c>
+      <c r="H30">
+        <v>560</v>
+      </c>
+      <c r="I30">
+        <v>470</v>
+      </c>
+      <c r="J30">
+        <v>533</v>
+      </c>
+      <c r="K30">
+        <v>391</v>
+      </c>
+      <c r="L30">
+        <v>421</v>
+      </c>
+      <c r="M30" s="2">
+        <f t="shared" si="2"/>
+        <v>3430.85</v>
+      </c>
+      <c r="N30">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32">
+        <v>300</v>
+      </c>
+      <c r="C32">
+        <v>300</v>
+      </c>
+      <c r="D32">
+        <v>200</v>
+      </c>
+      <c r="E32">
+        <v>237</v>
+      </c>
+      <c r="F32">
+        <v>128</v>
+      </c>
+      <c r="H32">
+        <v>600</v>
+      </c>
+      <c r="I32">
+        <v>540</v>
+      </c>
+      <c r="J32">
+        <v>680</v>
+      </c>
+      <c r="K32">
+        <v>475</v>
+      </c>
+      <c r="L32">
+        <v>600</v>
+      </c>
+      <c r="M32" s="2">
+        <f t="shared" si="2"/>
+        <v>4060</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12">
+      <c r="B34">
+        <f>B21/B$32</f>
+        <v>0.9365</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ref="C34:L34" si="3">C21/C$32</f>
+        <v>0.80666666666666664</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="3"/>
+        <v>0.82</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="3"/>
+        <v>0.89029535864978904</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="3"/>
+        <v>0.8125</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="3"/>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="3"/>
+        <v>0.83529411764705885</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="3"/>
+        <v>0.62526315789473685</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="3"/>
+        <v>0.64666666666666661</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12">
+      <c r="B35">
+        <f t="shared" ref="B35:C43" si="4">B22/B$32</f>
+        <v>0.95566666666666666</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="4"/>
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ref="D35:F35" si="5">D22/D$32</f>
+        <v>0.87</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="5"/>
+        <v>0.87763713080168781</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="5"/>
+        <v>0.796875</v>
+      </c>
+      <c r="H35">
+        <f t="shared" ref="H35:L35" si="6">H22/H$32</f>
+        <v>0.91333333333333333</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="6"/>
+        <v>0.89444444444444449</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="6"/>
+        <v>0.81617647058823528</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="6"/>
+        <v>0.84631578947368424</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="6"/>
+        <v>0.66833333333333333</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12">
+      <c r="B36">
+        <f t="shared" si="4"/>
+        <v>0.96016666666666672</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="4"/>
+        <v>0.85666666666666669</v>
+      </c>
+      <c r="D36">
+        <f t="shared" ref="D36:F36" si="7">D23/D$32</f>
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="7"/>
+        <v>0.89873417721518989</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="7"/>
+        <v>0.796875</v>
+      </c>
+      <c r="H36">
+        <f t="shared" ref="H36:L36" si="8">H23/H$32</f>
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="8"/>
+        <v>0.87962962962962965</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="8"/>
+        <v>0.79705882352941182</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="8"/>
+        <v>0.8610526315789474</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="8"/>
+        <v>0.66166666666666663</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12">
+      <c r="B37">
+        <f t="shared" si="4"/>
+        <v>0.9554999999999999</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="4"/>
+        <v>0.87333333333333329</v>
+      </c>
+      <c r="D37">
+        <f t="shared" ref="D37:F37" si="9">D24/D$32</f>
+        <v>0.87</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="9"/>
+        <v>0.89873417721518989</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="9"/>
+        <v>0.8203125</v>
+      </c>
+      <c r="H37">
+        <f t="shared" ref="H37:L37" si="10">H24/H$32</f>
+        <v>0.91333333333333333</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="10"/>
+        <v>0.85</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="10"/>
+        <v>0.66911764705882348</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="10"/>
+        <v>0.80421052631578949</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="10"/>
+        <v>0.65166666666666662</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12">
+      <c r="B38">
+        <f t="shared" si="4"/>
+        <v>0.95950000000000013</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="4"/>
+        <v>0.85666666666666669</v>
+      </c>
+      <c r="D38">
+        <f t="shared" ref="D38:F38" si="11">D25/D$32</f>
+        <v>0.875</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="11"/>
+        <v>0.89451476793248941</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="11"/>
+        <v>0.8203125</v>
+      </c>
+      <c r="H38">
+        <f t="shared" ref="H38:L38" si="12">H25/H$32</f>
+        <v>0.91</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="12"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="12"/>
+        <v>0.65588235294117647</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="12"/>
+        <v>0.84842105263157896</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="12"/>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12">
+      <c r="B39">
+        <f t="shared" si="4"/>
+        <v>0.95566666666666666</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="4"/>
+        <v>0.86</v>
+      </c>
+      <c r="D39">
+        <f t="shared" ref="D39:F39" si="13">D26/D$32</f>
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="13"/>
+        <v>0.88607594936708856</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="13"/>
+        <v>0.828125</v>
+      </c>
+      <c r="H39">
+        <f t="shared" ref="H39:L39" si="14">H26/H$32</f>
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="14"/>
+        <v>0.80555555555555558</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="14"/>
+        <v>0.63235294117647056</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="14"/>
+        <v>0.67789473684210522</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="14"/>
+        <v>0.68166666666666664</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12">
+      <c r="B40">
+        <f t="shared" si="4"/>
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="4"/>
+        <v>0.96333333333333337</v>
+      </c>
+      <c r="D40">
+        <f t="shared" ref="D40:F40" si="15">D27/D$32</f>
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="15"/>
+        <v>0.92827004219409281</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="15"/>
+        <v>0.8125</v>
+      </c>
+      <c r="H40">
+        <f t="shared" ref="H40:L40" si="16">H27/H$32</f>
+        <v>0.86333333333333329</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="16"/>
+        <v>0.79074074074074074</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="16"/>
+        <v>0.71029411764705885</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="16"/>
+        <v>0.84631578947368424</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="16"/>
+        <v>0.68500000000000005</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12">
+      <c r="B41">
+        <f t="shared" si="4"/>
+        <v>0.94450000000000012</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="4"/>
+        <v>0.87666666666666671</v>
+      </c>
+      <c r="D41">
+        <f t="shared" ref="D41:F41" si="17">D28/D$32</f>
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="17"/>
+        <v>0.89451476793248941</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="17"/>
+        <v>0.8203125</v>
+      </c>
+      <c r="H41">
+        <f t="shared" ref="H41:L41" si="18">H28/H$32</f>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="18"/>
+        <v>0.87037037037037035</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="18"/>
+        <v>0.84264705882352942</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="18"/>
+        <v>0.81263157894736837</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="18"/>
+        <v>0.69499999999999995</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12">
+      <c r="B42">
+        <f t="shared" si="4"/>
+        <v>0.95933333333333337</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="4"/>
+        <v>0.91333333333333333</v>
+      </c>
+      <c r="D42">
+        <f t="shared" ref="D42:F42" si="19">D29/D$32</f>
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="19"/>
+        <v>0.88607594936708856</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="19"/>
+        <v>0.7734375</v>
+      </c>
+      <c r="H42">
+        <f t="shared" ref="H42:L43" si="20">H29/H$32</f>
+        <v>0.95333333333333337</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="20"/>
+        <v>0.87037037037037035</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="20"/>
+        <v>0.82647058823529407</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="20"/>
+        <v>0.84</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="20"/>
+        <v>0.72499999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12">
+      <c r="B43">
+        <f t="shared" si="4"/>
+        <v>0.95616666666666672</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="4"/>
+        <v>0.93</v>
+      </c>
+      <c r="D43">
+        <f t="shared" ref="D43:F43" si="21">D30/D$32</f>
+        <v>0.88</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="21"/>
+        <v>0.88607594936708856</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="21"/>
+        <v>0.8125</v>
+      </c>
+      <c r="H43">
+        <f t="shared" ref="H43:K43" si="22">H30/H$32</f>
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="22"/>
+        <v>0.87037037037037035</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="22"/>
+        <v>0.7838235294117647</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="22"/>
+        <v>0.82315789473684209</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="20"/>
+        <v>0.70166666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>